<commit_message>
Committing Complete With All fixes to GIT
</commit_message>
<xml_diff>
--- a/input/MDM_Output.xlsx
+++ b/input/MDM_Output.xlsx
@@ -1,55 +1,64 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Git\Batch Run Mendix\Mendix_BatchRun\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0276A84C-8779-4E59-BEED-97E9A8329E91}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAA0EB1-5E9F-4C34-A00C-4FF3C03A45D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{D4118D02-8BFE-451B-B043-4051382126A2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OutputTestData" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Login</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Test_Case</t>
   </si>
   <si>
-    <t>RequestId</t>
+    <t>Global_ID</t>
   </si>
   <si>
     <t>Material_Number_AH1</t>
   </si>
   <si>
-    <t>Global_ID</t>
+    <t>Mendix_User</t>
+  </si>
+  <si>
+    <t>Syndication_Status</t>
+  </si>
+  <si>
+    <t>UFT_User</t>
+  </si>
+  <si>
+    <t>DummyRow</t>
+  </si>
+  <si>
+    <t>14.Create_Vendor_with_Questionnaire_only_Global_SAP.xml</t>
+  </si>
+  <si>
+    <t>505375</t>
+  </si>
+  <si>
+    <t>1000115723</t>
+  </si>
+  <si>
+    <t>MDVM_BE01_LDR</t>
+  </si>
+  <si>
+    <t>Syndication Not Done</t>
+  </si>
+  <si>
+    <t>SAP</t>
   </si>
 </sst>
 </file>
@@ -59,7 +68,7 @@
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -400,16 +409,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B70F225-A30D-4F52-9B14-3308B84399D9}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,61 +429,56 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341B2C85-10B2-4C56-B82E-91FBCC369749}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DF7856-3998-41FA-8B35-61274A6D7BE4}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6FB5C0-FAD4-4FFE-AA29-8493093F9A3D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B5A373-7273-4139-B79C-D17FB260CF06}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Committing complete fixes to of enhancements to GIT
</commit_message>
<xml_diff>
--- a/input/MDM_Output.xlsx
+++ b/input/MDM_Output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Git\Batch Run Mendix\Mendix_BatchRun\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAA0EB1-5E9F-4C34-A00C-4FF3C03A45D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C75D91E-958B-4EF0-A8CD-E1358DAB240B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -413,7 +413,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D11" sqref="D11:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>